<commit_message>
Scrum 2 week 2
</commit_message>
<xml_diff>
--- a/scrum/Scrum_week2.xlsx
+++ b/scrum/Scrum_week2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Wat heb ik gedaan?</t>
   </si>
@@ -54,15 +54,6 @@
     <t>Git wou niet pushen, goesting was ver te zoeken</t>
   </si>
   <si>
-    <t>remote van git,</t>
-  </si>
-  <si>
-    <t>template make</t>
-  </si>
-  <si>
-    <t>scrum+to do lijst - trigger + stored procedures</t>
-  </si>
-  <si>
     <t>testdata afwerken , testen git met HTML project,nazicht git handleiding, html5 tutorials</t>
   </si>
   <si>
@@ -70,6 +61,21 @@
   </si>
   <si>
     <t>Documentatie git afwerken, Git in orde maken, logo maken</t>
+  </si>
+  <si>
+    <t>scrum+to do lijst - trigger + stored procedures, festivals aanpassen,groepen aanpassen</t>
+  </si>
+  <si>
+    <t>template maken, details groepen</t>
+  </si>
+  <si>
+    <t>remote van git,home</t>
+  </si>
+  <si>
+    <t>template maken, festival detail +festival detail aanpassen,groepen detail aanpassen</t>
+  </si>
+  <si>
+    <t>template maken,festivals, groepen</t>
   </si>
 </sst>
 </file>
@@ -478,7 +484,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -486,6 +492,7 @@
     <col min="2" max="2" width="32.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.375" customWidth="1"/>
     <col min="4" max="4" width="36.625" customWidth="1"/>
+    <col min="5" max="5" width="22.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -509,7 +516,7 @@
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -517,11 +524,11 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="71.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -529,11 +536,11 @@
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="71.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -547,7 +554,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.25">
@@ -555,11 +562,11 @@
         <v>7</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>